<commit_message>
Add boisson for spec test
</commit_message>
<xml_diff>
--- a/documentation/specTestSpringwater.xlsx
+++ b/documentation/specTestSpringwater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\springwater\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDD526D-2351-4ECF-8A45-DB6C07D7E225}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922C1DDA-323C-4634-B5C1-637264498A59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="143">
   <si>
     <t>Cluster id</t>
   </si>
@@ -306,39 +306,15 @@
     <t>PROFILC1T1</t>
   </si>
   <si>
-    <t>https://beerreviews.srvz-webapp.he-arc.ch/beers/1/</t>
-  </si>
-  <si>
-    <t>Entrer valeurs:</t>
-  </si>
-  <si>
     <t>COMMC1T2</t>
   </si>
   <si>
     <t>COMMC2T1</t>
   </si>
   <si>
-    <t>https://beerreviews.srvz-webapp.he-arc.ch/users/profile</t>
-  </si>
-  <si>
-    <t>Vérifier que les commentaires des tests précédents s'affichent</t>
-  </si>
-  <si>
     <t>COMMC3T1</t>
   </si>
   <si>
-    <t>Cliquer sur le lien d'une bière notée précédamment</t>
-  </si>
-  <si>
-    <t>Retenir le commentaire et note initiale faite avec notre compte</t>
-  </si>
-  <si>
-    <t>secondTest</t>
-  </si>
-  <si>
-    <t>Vérifier que le nouveau commentaire et note ont remplacé l'ancien</t>
-  </si>
-  <si>
     <t>CHARGEC1T1</t>
   </si>
   <si>
@@ -448,13 +424,46 @@
   </si>
   <si>
     <t>Constater qu'une liste de boisson est proposée</t>
+  </si>
+  <si>
+    <t>BOIS2T1</t>
+  </si>
+  <si>
+    <t>BOIS3T1</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton modifier d'une boisson</t>
+  </si>
+  <si>
+    <t>Modifier les champs</t>
+  </si>
+  <si>
+    <t>Constater que le nom et la description de la bière ont bien changer</t>
+  </si>
+  <si>
+    <t>BOIS4T1</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton détail d'une boissone</t>
+  </si>
+  <si>
+    <t>Constater que les détails de la boisson sont affichées</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton supprimer d'une boisson</t>
+  </si>
+  <si>
+    <t>Confirmer la suppression</t>
+  </si>
+  <si>
+    <t>Constater que la boisson a bien été supprimée</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -533,6 +542,12 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -648,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -676,6 +691,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2172,7 +2188,7 @@
     </row>
     <row r="13" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>36</v>
@@ -3179,10 +3195,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R1048573"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3808,6 +3824,9 @@
       <c r="A77" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="D77" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="M77" s="8"/>
     </row>
     <row r="78" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4029,7 +4048,9 @@
       <c r="A108" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D108" s="2"/>
+      <c r="D108" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="M108" s="8"/>
     </row>
     <row r="109" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4103,7 +4124,9 @@
       <c r="A119" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D119" s="2"/>
+      <c r="D119" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="M119" s="8"/>
     </row>
     <row r="120" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4144,7 +4167,7 @@
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
@@ -4166,7 +4189,7 @@
         <v>43</v>
       </c>
       <c r="E127" s="22" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F127" s="22" t="s">
         <v>13</v>
@@ -4195,27 +4218,27 @@
         <v>56</v>
       </c>
       <c r="H130" s="11" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="M130" s="8"/>
     </row>
     <row r="131" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="24" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D131" s="2"/>
       <c r="E131" s="23" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F131" s="23" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G131" s="2"/>
       <c r="M131" s="8"/>
     </row>
     <row r="132" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="24" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
@@ -4224,7 +4247,7 @@
     </row>
     <row r="133" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="25" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="13"/>
@@ -4248,8 +4271,8 @@
       </c>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
-      <c r="D137" s="5" t="s">
-        <v>130</v>
+      <c r="D137" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
@@ -4267,9 +4290,7 @@
     </row>
     <row r="139" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="7"/>
-      <c r="D139" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="D139" s="9"/>
       <c r="E139" s="9" t="s">
         <v>87</v>
       </c>
@@ -4291,13 +4312,13 @@
         <v>56</v>
       </c>
       <c r="H141" s="26" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="M141" s="8"/>
     </row>
     <row r="142" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="24" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -4333,8 +4354,8 @@
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
-      <c r="D147" s="5" t="s">
-        <v>130</v>
+      <c r="D147" s="27" t="s">
+        <v>133</v>
       </c>
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
@@ -4358,8 +4379,12 @@
       <c r="E149" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F149" s="9"/>
-      <c r="G149" s="9"/>
+      <c r="F149" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="G149" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="M149" s="8"/>
     </row>
     <row r="150" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4379,256 +4404,336 @@
       <c r="A152" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E152" s="11" t="s">
-        <v>96</v>
+      <c r="E152" s="26" t="s">
+        <v>130</v>
       </c>
       <c r="M152" s="8"/>
     </row>
     <row r="153" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B153" s="13"/>
-      <c r="C153" s="13"/>
-      <c r="D153" s="13"/>
-      <c r="E153" s="13"/>
-      <c r="F153" s="13"/>
-      <c r="G153" s="13"/>
-      <c r="H153" s="13"/>
-      <c r="I153" s="13"/>
-      <c r="J153" s="13"/>
-      <c r="K153" s="13"/>
-      <c r="L153" s="13"/>
-      <c r="M153" s="14"/>
+      <c r="A153" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E153" s="26"/>
+      <c r="M153" s="8"/>
     </row>
     <row r="154" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="2"/>
+      <c r="A154" s="24" t="s">
+        <v>135</v>
+      </c>
       <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
+      <c r="F154" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G154" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="M154" s="8"/>
     </row>
     <row r="155" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="2"/>
+      <c r="A155" s="24" t="s">
+        <v>128</v>
+      </c>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
+      <c r="M155" s="8"/>
     </row>
     <row r="156" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E156" s="26"/>
+      <c r="M156" s="8"/>
+    </row>
+    <row r="157" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="10"/>
+      <c r="E157" s="26"/>
+      <c r="M157" s="8"/>
+    </row>
+    <row r="158" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="12"/>
+      <c r="B158" s="13"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="13"/>
+      <c r="G158" s="13"/>
+      <c r="H158" s="13"/>
+      <c r="I158" s="13"/>
+      <c r="J158" s="13"/>
+      <c r="K158" s="13"/>
+      <c r="L158" s="13"/>
+      <c r="M158" s="14"/>
+    </row>
+    <row r="159" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+    </row>
+    <row r="160" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+    </row>
+    <row r="161" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B156" s="4"/>
-      <c r="C156" s="4"/>
-      <c r="D156" s="5" t="s">
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
+      <c r="H161" s="4"/>
+      <c r="I161" s="4"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
+      <c r="L161" s="4"/>
+      <c r="M161" s="6"/>
+    </row>
+    <row r="162" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="7"/>
+      <c r="M162" s="8"/>
+    </row>
+    <row r="163" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="7"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F163" s="9"/>
+      <c r="M163" s="8"/>
+    </row>
+    <row r="164" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="7"/>
+      <c r="M164" s="8"/>
+    </row>
+    <row r="165" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E165" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="E156" s="4"/>
-      <c r="F156" s="4"/>
-      <c r="G156" s="4"/>
-      <c r="H156" s="4"/>
-      <c r="I156" s="4"/>
-      <c r="J156" s="4"/>
-      <c r="K156" s="4"/>
-      <c r="L156" s="4"/>
-      <c r="M156" s="6"/>
-    </row>
-    <row r="157" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="7"/>
-      <c r="M157" s="8"/>
-    </row>
-    <row r="158" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="7"/>
-      <c r="D158" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E158" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F158" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G158" s="9" t="s">
+      <c r="M165" s="8"/>
+    </row>
+    <row r="166" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="M166" s="8"/>
+    </row>
+    <row r="167" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="M167" s="8"/>
+    </row>
+    <row r="168" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="10"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+      <c r="M168" s="8"/>
+    </row>
+    <row r="169" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="12"/>
+      <c r="B169" s="13"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="13"/>
+      <c r="G169" s="13"/>
+      <c r="H169" s="13"/>
+      <c r="I169" s="13"/>
+      <c r="J169" s="13"/>
+      <c r="K169" s="13"/>
+      <c r="L169" s="13"/>
+      <c r="M169" s="14"/>
+    </row>
+    <row r="170" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="2"/>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="2"/>
+    </row>
+    <row r="172" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B172" s="4"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="4"/>
+      <c r="L172" s="4"/>
+      <c r="M172" s="6"/>
+    </row>
+    <row r="173" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="7"/>
+      <c r="M173" s="8"/>
+    </row>
+    <row r="174" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="7"/>
+      <c r="D174" s="9"/>
+      <c r="E174" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="M158" s="8"/>
-    </row>
-    <row r="159" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="7"/>
-      <c r="M159" s="8"/>
-    </row>
-    <row r="160" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="10" t="s">
+      <c r="F174" s="9"/>
+      <c r="M174" s="8"/>
+    </row>
+    <row r="175" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D160" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M160" s="8"/>
-    </row>
-    <row r="161" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="10" t="s">
+      <c r="M175" s="8"/>
+    </row>
+    <row r="176" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G161" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="M161" s="8"/>
-      <c r="Q161" s="2"/>
-      <c r="R161" s="2"/>
-    </row>
-    <row r="162" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="M162" s="8"/>
-      <c r="Q162" s="2"/>
-      <c r="R162" s="2"/>
-    </row>
-    <row r="163" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="M163" s="8"/>
-      <c r="Q163" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R163" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F164" s="2">
-        <v>3</v>
-      </c>
-      <c r="M164" s="8"/>
-      <c r="Q164" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R164" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="165" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B165" s="13"/>
-      <c r="C165" s="13"/>
-      <c r="D165" s="13"/>
-      <c r="E165" s="13"/>
-      <c r="F165" s="13"/>
-      <c r="G165" s="13"/>
-      <c r="H165" s="13"/>
-      <c r="I165" s="13"/>
-      <c r="J165" s="13"/>
-      <c r="K165" s="13"/>
-      <c r="L165" s="13"/>
-      <c r="M165" s="14"/>
-      <c r="Q165" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R165" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="168" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="3" t="s">
+      <c r="E176" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="M176" s="8"/>
+      <c r="Q176" s="2"/>
+      <c r="R176" s="2"/>
+    </row>
+    <row r="177" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="M177" s="8"/>
+      <c r="Q177" s="2"/>
+      <c r="R177" s="2"/>
+    </row>
+    <row r="178" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M178" s="8"/>
+      <c r="Q178" s="2"/>
+      <c r="R178" s="2"/>
+    </row>
+    <row r="179" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
+      <c r="M179" s="8"/>
+      <c r="Q179" s="2"/>
+      <c r="R179" s="2"/>
+    </row>
+    <row r="180" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="12"/>
+      <c r="B180" s="13"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="13"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="13"/>
+      <c r="J180" s="13"/>
+      <c r="K180" s="13"/>
+      <c r="L180" s="13"/>
+      <c r="M180" s="14"/>
+      <c r="Q180" s="2"/>
+      <c r="R180" s="2"/>
+    </row>
+    <row r="183" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B168" s="4"/>
-      <c r="C168" s="4"/>
-      <c r="D168" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E168" s="4"/>
-      <c r="F168" s="4"/>
-      <c r="G168" s="4"/>
-      <c r="H168" s="4"/>
-      <c r="I168" s="4"/>
-      <c r="J168" s="4"/>
-      <c r="K168" s="4"/>
-      <c r="L168" s="4"/>
-      <c r="M168" s="6"/>
-    </row>
-    <row r="169" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="7"/>
-      <c r="M169" s="8"/>
-    </row>
-    <row r="170" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="7"/>
-      <c r="D170" s="9" t="s">
+      <c r="B183" s="4"/>
+      <c r="C183" s="4"/>
+      <c r="D183" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
+      <c r="H183" s="4"/>
+      <c r="I183" s="4"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="4"/>
+      <c r="L183" s="4"/>
+      <c r="M183" s="6"/>
+    </row>
+    <row r="184" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="7"/>
+      <c r="M184" s="8"/>
+    </row>
+    <row r="185" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="7"/>
+      <c r="D185" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E170" s="9"/>
-      <c r="F170" s="9"/>
-      <c r="G170" s="9"/>
-      <c r="M170" s="8"/>
-    </row>
-    <row r="171" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="7"/>
-      <c r="M171" s="8"/>
-    </row>
-    <row r="172" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="M172" s="8"/>
-    </row>
-    <row r="173" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="10"/>
-      <c r="D173" s="2"/>
-      <c r="E173" s="2"/>
-      <c r="F173" s="2"/>
-      <c r="G173" s="2"/>
-      <c r="M173" s="8"/>
-    </row>
-    <row r="174" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="10"/>
-      <c r="E174" s="2"/>
-      <c r="F174" s="2"/>
-      <c r="M174" s="8"/>
-    </row>
-    <row r="175" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B175" s="13"/>
-      <c r="C175" s="13"/>
-      <c r="D175" s="13"/>
-      <c r="E175" s="13"/>
-      <c r="F175" s="13"/>
-      <c r="G175" s="13"/>
-      <c r="H175" s="13"/>
-      <c r="I175" s="13"/>
-      <c r="J175" s="13"/>
-      <c r="K175" s="13"/>
-      <c r="L175" s="13"/>
-      <c r="M175" s="14"/>
-    </row>
-    <row r="176" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="9"/>
+      <c r="G185" s="9"/>
+      <c r="M185" s="8"/>
+    </row>
+    <row r="186" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="7"/>
+      <c r="M186" s="8"/>
+    </row>
+    <row r="187" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="M187" s="8"/>
+    </row>
+    <row r="188" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="10"/>
+      <c r="D188" s="2"/>
+      <c r="E188" s="2"/>
+      <c r="F188" s="2"/>
+      <c r="G188" s="2"/>
+      <c r="M188" s="8"/>
+    </row>
+    <row r="189" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="10"/>
+      <c r="E189" s="2"/>
+      <c r="F189" s="2"/>
+      <c r="M189" s="8"/>
+    </row>
+    <row r="190" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B190" s="13"/>
+      <c r="C190" s="13"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
+      <c r="F190" s="13"/>
+      <c r="G190" s="13"/>
+      <c r="H190" s="13"/>
+      <c r="I190" s="13"/>
+      <c r="J190" s="13"/>
+      <c r="K190" s="13"/>
+      <c r="L190" s="13"/>
+      <c r="M190" s="14"/>
+    </row>
+    <row r="191" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5416,32 +5521,36 @@
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048556" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048557" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048558" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048559" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048560" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048561" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048562" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048563" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048564" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048565" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048566" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048567" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048568" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048569" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048570" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H141" r:id="rId1" display="https://beerreviews.srvz-webapp.he-arc.ch/beers/1/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="E152" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="G161" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E152" r:id="rId2" display="https://beerreviews.srvz-webapp.he-arc.ch/users/profile" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E176" r:id="rId3" display="https://beerreviews.srvz-webapp.he-arc.ch/beers/1/" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E165" r:id="rId4" display="https://beerreviews.srvz-webapp.he-arc.ch/beers/1/" xr:uid="{04B77A97-ABEF-47C1-8AC8-845D9C8943CF}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5467,48 +5576,48 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D4" s="20"/>
     </row>
@@ -5517,107 +5626,107 @@
         <v>91</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -5627,50 +5736,50 @@
         <v>86</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D20" s="20"/>
     </row>

</xml_diff>